<commit_message>
Final Update for authortest
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10560" windowHeight="1410" firstSheet="13" activeTab="19"/>
+    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
@@ -182,7 +182,7 @@
     <t>RQ-443</t>
   </si>
   <si>
-    <t>TC-528</t>
+    <t>TC-517</t>
   </si>
   <si>
     <t>requirementId</t>
@@ -1501,8 +1501,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1714,7 +1714,7 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2508,7 +2508,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
author test is done
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="13" activeTab="14"/>
+    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
@@ -1392,8 +1392,8 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1501,7 +1501,7 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2508,7 +2508,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
relevant files added for Test plan tab
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="8" activeTab="11"/>
+    <workbookView windowWidth="19200" windowHeight="6080" firstSheet="13" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
@@ -36,14 +36,6 @@
     <sheet name="tc071" sheetId="26" r:id="rId27"/>
     <sheet name="tc072" sheetId="27" r:id="rId28"/>
     <sheet name="tc073" sheetId="30" r:id="rId29"/>
-    <sheet name="tc041" sheetId="31" r:id="rId30"/>
-    <sheet name="tc051" sheetId="32" r:id="rId31"/>
-    <sheet name="tc052" sheetId="33" r:id="rId32"/>
-    <sheet name="tc055" sheetId="34" r:id="rId33"/>
-    <sheet name="tc059" sheetId="35" r:id="rId34"/>
-    <sheet name="tc060" sheetId="36" r:id="rId35"/>
-    <sheet name="tc066" sheetId="37" r:id="rId36"/>
-    <sheet name="tc067" sheetId="38" r:id="rId37"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="61">
   <si>
     <t>Epic</t>
   </si>
@@ -179,10 +171,7 @@
     <t>TestcaseId</t>
   </si>
   <si>
-    <t>RQ-443</t>
-  </si>
-  <si>
-    <t>TC-517</t>
+    <t>TC-369</t>
   </si>
   <si>
     <t>requirementId</t>
@@ -206,7 +195,7 @@
     <t>testcaseId</t>
   </si>
   <si>
-    <t>TC-529</t>
+    <t>TC-458</t>
   </si>
   <si>
     <t>Req-Id</t>
@@ -242,9 +231,6 @@
     <t>TC-453</t>
   </si>
   <si>
-    <t>TC-458</t>
-  </si>
-  <si>
     <t>RQ-438</t>
   </si>
   <si>
@@ -252,45 +238,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>rqName</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>qaUser</t>
-  </si>
-  <si>
-    <t>preCondition</t>
-  </si>
-  <si>
-    <t>New_tc</t>
-  </si>
-  <si>
-    <t>Na</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>Vivek Rajput</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>rQtitle</t>
-  </si>
-  <si>
-    <t>SET Drive</t>
-  </si>
-  <si>
-    <t>tcId</t>
   </si>
 </sst>
 </file>
@@ -303,23 +250,10 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF475467"/>
-      <name val="Arial"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -785,19 +719,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -806,138 +749,127 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1392,8 +1324,8 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1430,30 +1362,30 @@
   </cols>
   <sheetData>
     <row r="1" ht="29" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1502,25 +1434,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1544,109 +1476,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="A1:D2 C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" ht="29" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="A1:D2 C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="3"/>
-  <sheetData>
-    <row r="1" ht="29" spans="1:4">
-      <c r="A1" s="4" t="s">
+    <row r="2" ht="29" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" ht="29" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" ht="29" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" ht="29" spans="1:4">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
-  <sheetData>
-    <row r="1" ht="29" spans="1:5">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="2" ht="29" spans="1:5">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1668,7 +1600,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1715,25 +1647,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1765,10 +1697,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1813,10 +1745,10 @@
         <v>30</v>
       </c>
       <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1833,7 +1765,7 @@
         <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1864,7 +1796,7 @@
         <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -1881,7 +1813,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1898,8 +1830,8 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="5"/>
@@ -1911,22 +1843,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>55</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>56</v>
-      </c>
-      <c r="F1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1934,7 +1866,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -1961,7 +1893,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1971,19 +1903,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2008,12 +1940,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2038,12 +1970,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2068,18 +2000,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2105,37 +2037,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>62</v>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>62</v>
+      <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2343,318 +2275,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="6"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="6"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -2748,7 +2368,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
tc003 updated for author
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6080" firstSheet="18" activeTab="23"/>
+    <workbookView windowWidth="19200" windowHeight="6800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="62">
   <si>
     <t>Epic</t>
   </si>
@@ -102,7 +102,10 @@
     <t>Label Name</t>
   </si>
   <si>
-    <t>Epic Count</t>
+    <t>project name</t>
+  </si>
+  <si>
+    <t>STG- PulseCodeOnAzureCloud</t>
   </si>
   <si>
     <t/>
@@ -250,7 +253,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -262,6 +265,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <charset val="134"/>
     </font>
     <font>
@@ -719,157 +728,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1262,7 +1272,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1293,13 +1303,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1307,7 +1317,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1332,12 +1342,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1369,10 +1379,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1380,13 +1390,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1408,18 +1418,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1441,18 +1451,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1477,12 +1487,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1510,10 +1520,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" ht="29" spans="1:4">
@@ -1521,13 +1531,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1555,13 +1565,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" ht="29" spans="1:5">
@@ -1569,16 +1579,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1600,12 +1610,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1654,18 +1664,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1697,10 +1707,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1708,10 +1718,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1742,13 +1752,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1756,16 +1766,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1793,10 +1803,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -1807,13 +1817,13 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1830,7 +1840,7 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -1843,30 +1853,30 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -1904,18 +1914,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1940,12 +1950,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1970,12 +1980,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2000,18 +2010,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2044,13 +2054,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2058,16 +2068,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2081,8 +2091,8 @@
   <sheetPr/>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -2093,180 +2103,180 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2">
-        <v>11</v>
+      <c r="A2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2315,7 +2325,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2326,7 +2336,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2353,7 +2363,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2408,13 +2418,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2425,7 +2435,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2447,12 +2457,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Updation for Headless
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6080" firstSheet="18" activeTab="23"/>
+    <workbookView windowWidth="19200" windowHeight="6080" firstSheet="13" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
@@ -36,6 +36,13 @@
     <sheet name="tc071" sheetId="26" r:id="rId27"/>
     <sheet name="tc072" sheetId="27" r:id="rId28"/>
     <sheet name="tc073" sheetId="30" r:id="rId29"/>
+    <sheet name="tc041" sheetId="31" r:id="rId30"/>
+    <sheet name="tc051" sheetId="32" r:id="rId31"/>
+    <sheet name="tc052" sheetId="33" r:id="rId32"/>
+    <sheet name="tc059" sheetId="34" r:id="rId33"/>
+    <sheet name="tc066" sheetId="35" r:id="rId34"/>
+    <sheet name="tc067" sheetId="36" r:id="rId35"/>
+    <sheet name="tc060" sheetId="37" r:id="rId36"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="76">
   <si>
     <t>Epic</t>
   </si>
@@ -84,7 +91,7 @@
     <t>Feature Mohit</t>
   </si>
   <si>
-    <t>RQ-469</t>
+    <t>RQ-679</t>
   </si>
   <si>
     <t>Tc-08</t>
@@ -102,7 +109,10 @@
     <t>Label Name</t>
   </si>
   <si>
-    <t>Epic Count</t>
+    <t>project name</t>
+  </si>
+  <si>
+    <t>STG- PulseCodeOnAzureCloud</t>
   </si>
   <si>
     <t/>
@@ -171,7 +181,7 @@
     <t>TestcaseId</t>
   </si>
   <si>
-    <t>TC-369</t>
+    <t>TC-477</t>
   </si>
   <si>
     <t>requirementId</t>
@@ -195,42 +205,45 @@
     <t>testcaseId</t>
   </si>
   <si>
+    <t>TC-464</t>
+  </si>
+  <si>
+    <t>Req-Id</t>
+  </si>
+  <si>
+    <t>Expected-Pagination</t>
+  </si>
+  <si>
+    <t>tcid</t>
+  </si>
+  <si>
+    <t>tcName</t>
+  </si>
+  <si>
+    <t>TC-09</t>
+  </si>
+  <si>
+    <t>testCase-Id</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>TC-437</t>
+  </si>
+  <si>
     <t>TC-458</t>
   </si>
   <si>
-    <t>Req-Id</t>
-  </si>
-  <si>
-    <t>Expected-Pagination</t>
-  </si>
-  <si>
-    <t>tcid</t>
-  </si>
-  <si>
-    <t>tcName</t>
-  </si>
-  <si>
-    <t>TC-09</t>
-  </si>
-  <si>
-    <t>testCase-Id</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>automation</t>
-  </si>
-  <si>
-    <t>TC-453</t>
-  </si>
-  <si>
     <t>RQ-438</t>
   </si>
   <si>
@@ -238,6 +251,45 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>rqName</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>qaUser</t>
+  </si>
+  <si>
+    <t>preCondition</t>
+  </si>
+  <si>
+    <t>New_tc</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Vivek Rajput</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>rQtitle</t>
+  </si>
+  <si>
+    <t>SET Drive</t>
+  </si>
+  <si>
+    <t>tcId</t>
   </si>
 </sst>
 </file>
@@ -250,7 +302,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -259,9 +311,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF475467"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0BA5EC"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -719,157 +796,161 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1192,7 +1273,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="6"/>
@@ -1227,7 +1308,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
@@ -1262,7 +1343,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1293,13 +1374,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1307,7 +1388,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -1332,12 +1413,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1362,32 +1443,32 @@
   </cols>
   <sheetData>
     <row r="1" ht="29" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1401,25 +1482,25 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1433,26 +1514,26 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1476,109 +1557,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" ht="29" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" ht="29" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="A1:D2 C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="3"/>
-  <sheetData>
-    <row r="1" ht="29" spans="1:4">
-      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" ht="29" spans="1:5">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" ht="29" spans="1:4">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" ht="29" spans="1:5">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
-  <sheetData>
-    <row r="1" ht="29" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" ht="29" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>43</v>
+      <c r="E2" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1600,12 +1681,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1646,26 +1727,26 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1697,10 +1778,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1708,10 +1789,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -1742,13 +1823,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1756,16 +1837,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1793,10 +1874,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -1807,13 +1888,13 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1830,8 +1911,8 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="5"/>
@@ -1842,42 +1923,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="4">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1893,7 +1974,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A1" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1903,19 +1984,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>45</v>
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>46</v>
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1940,12 +2021,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1970,12 +2051,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2000,18 +2081,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2026,7 +2107,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -2037,37 +2118,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>60</v>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>60</v>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2082,7 +2163,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -2093,180 +2174,467 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2">
-        <v>11</v>
+      <c r="A2" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="3" max="3" width="9.25454545454545" customWidth="1"/>
+    <col min="6" max="6" width="10.2545454545455" customWidth="1"/>
+    <col min="7" max="7" width="10.7545454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="6" max="6" width="10.2545454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2315,7 +2683,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2326,7 +2694,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2353,7 +2721,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2408,13 +2776,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2425,7 +2793,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2447,12 +2815,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TC05,TC022 Added for executeTab
</commit_message>
<xml_diff>
--- a/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
+++ b/testData/authorTestTabTestData/authorTestCaseTab_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6080" firstSheet="13" activeTab="14"/>
+    <workbookView windowWidth="19200" windowHeight="6080" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="AddTest" sheetId="2" r:id="rId1"/>
@@ -297,12 +297,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -325,6 +325,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
     </font>
@@ -332,7 +339,7 @@
       <sz val="9"/>
       <color rgb="FF0BA5EC"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -789,152 +796,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -943,6 +950,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,7 +959,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1300,7 +1308,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
@@ -1398,7 +1406,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1"/>
@@ -1507,7 +1515,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1904,7 +1912,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75454545454545" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="5"/>
@@ -1915,42 +1923,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>3</v>
       </c>
     </row>
@@ -1966,7 +1974,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -2155,7 +2163,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -2166,7 +2174,7 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2640,8 +2648,8 @@
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>

</xml_diff>